<commit_message>
new version of lake indicators in accordance with WFD2ECA v. 2.0
</commit_message>
<xml_diff>
--- a/indicators/NO_WPPB_001/metadata.xlsx
+++ b/indicators/NO_WPPB_001/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanno.sandvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7021CC-C3A9-4A91-A467-F1D2A316E4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0737C6C-E2A1-4860-85BC-9C7C6DC7270C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -702,9 +702,6 @@
     <t>First complete version</t>
   </si>
   <si>
-    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_WCHL_001</t>
-  </si>
-  <si>
     <t>NO_WPPB_001</t>
   </si>
   <si>
@@ -712,6 +709,9 @@
   </si>
   <si>
     <t>Scale - Transform - Aggregate (area-weighted arithmetic mean) - Truncate</t>
+  </si>
+  <si>
+    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_WPPB_001</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>198</v>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>200</v>
@@ -1384,7 +1384,7 @@
         <v>184</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>188</v>
@@ -1412,7 +1412,7 @@
         <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>197</v>

</xml_diff>